<commit_message>
Implemented jump, working on Dodge
</commit_message>
<xml_diff>
--- a/Documents/Timesheet.xlsx
+++ b/Documents/Timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Project Dungeon Escape - Timetable</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>Implemented Jump, started working on dodge</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +396,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" s="3">
         <f>(SUM(C4:C8)-SUM(B4:B8))*24</f>
-        <v>1.5</v>
+        <v>2.1333333333333311</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -434,8 +437,21 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="1">
+        <v>42722</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>

</xml_diff>